<commit_message>
Updated reports, updated spreadsheets and added and updated graphics
</commit_message>
<xml_diff>
--- a/extra_baselines/rem_open_access.xlsx
+++ b/extra_baselines/rem_open_access.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="0" windowWidth="22080" windowHeight="15320" tabRatio="500" activeTab="1"/>
@@ -10562,19 +10562,17 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="D269:E269"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B229:C229"/>
-    <mergeCell ref="B269:C269"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="F149:G149"/>
-    <mergeCell ref="F189:G189"/>
-    <mergeCell ref="F229:G229"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D189:E189"/>
-    <mergeCell ref="D229:E229"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F108:G108"/>
@@ -10582,18 +10580,20 @@
     <mergeCell ref="H148:I148"/>
     <mergeCell ref="H188:I188"/>
     <mergeCell ref="H228:I228"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="B38:C38"/>
     <mergeCell ref="H268:I268"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="F149:G149"/>
+    <mergeCell ref="F189:G189"/>
+    <mergeCell ref="F229:G229"/>
+    <mergeCell ref="D269:E269"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B229:C229"/>
+    <mergeCell ref="B269:C269"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D189:E189"/>
+    <mergeCell ref="D229:E229"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -10609,10 +10609,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A18" sqref="A18"/>
-      <selection pane="topRight" activeCell="I390" sqref="I390"/>
+      <selection pane="topRight" activeCell="F255" sqref="F255:I257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -27566,18 +27566,37 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="P295:Q295"/>
-    <mergeCell ref="L167:M167"/>
-    <mergeCell ref="L210:M210"/>
-    <mergeCell ref="L253:M253"/>
-    <mergeCell ref="L296:M296"/>
-    <mergeCell ref="P209:Q209"/>
-    <mergeCell ref="P252:Q252"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="F126:G126"/>
-    <mergeCell ref="H126:I126"/>
-    <mergeCell ref="J126:K126"/>
-    <mergeCell ref="L126:M126"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="P126:Q126"/>
+    <mergeCell ref="P166:Q166"/>
+    <mergeCell ref="F210:G210"/>
+    <mergeCell ref="F253:G253"/>
+    <mergeCell ref="F296:G296"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N167:O167"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N85:O85"/>
+    <mergeCell ref="N126:O126"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="H296:I296"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J167:K167"/>
+    <mergeCell ref="L85:M85"/>
+    <mergeCell ref="H253:I253"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H167:I167"/>
+    <mergeCell ref="H210:I210"/>
     <mergeCell ref="D296:E296"/>
     <mergeCell ref="B210:C210"/>
     <mergeCell ref="B253:C253"/>
@@ -27594,40 +27613,21 @@
     <mergeCell ref="D167:E167"/>
     <mergeCell ref="D210:E210"/>
     <mergeCell ref="D253:E253"/>
-    <mergeCell ref="H296:I296"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J167:K167"/>
-    <mergeCell ref="L85:M85"/>
-    <mergeCell ref="H253:I253"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="F126:G126"/>
+    <mergeCell ref="H126:I126"/>
+    <mergeCell ref="J126:K126"/>
+    <mergeCell ref="L126:M126"/>
+    <mergeCell ref="P295:Q295"/>
+    <mergeCell ref="L167:M167"/>
+    <mergeCell ref="L210:M210"/>
+    <mergeCell ref="L253:M253"/>
+    <mergeCell ref="L296:M296"/>
+    <mergeCell ref="P209:Q209"/>
+    <mergeCell ref="P252:Q252"/>
     <mergeCell ref="N210:O210"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H167:I167"/>
-    <mergeCell ref="H210:I210"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N85:O85"/>
-    <mergeCell ref="N126:O126"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
     <mergeCell ref="N253:O253"/>
     <mergeCell ref="N296:O296"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="F210:G210"/>
-    <mergeCell ref="F253:G253"/>
-    <mergeCell ref="F296:G296"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N167:O167"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="P126:Q126"/>
-    <mergeCell ref="P166:Q166"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -35685,6 +35685,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D189:E189"/>
+    <mergeCell ref="D229:E229"/>
+    <mergeCell ref="D269:E269"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="F149:G149"/>
+    <mergeCell ref="F189:G189"/>
+    <mergeCell ref="B229:C229"/>
+    <mergeCell ref="B269:C269"/>
+    <mergeCell ref="F229:G229"/>
     <mergeCell ref="H188:I188"/>
     <mergeCell ref="H228:I228"/>
     <mergeCell ref="H268:I268"/>
@@ -35698,25 +35717,6 @@
     <mergeCell ref="H74:I74"/>
     <mergeCell ref="H110:I110"/>
     <mergeCell ref="H148:I148"/>
-    <mergeCell ref="D189:E189"/>
-    <mergeCell ref="D229:E229"/>
-    <mergeCell ref="D269:E269"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="F149:G149"/>
-    <mergeCell ref="F189:G189"/>
-    <mergeCell ref="B229:C229"/>
-    <mergeCell ref="B269:C269"/>
-    <mergeCell ref="F229:G229"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B149:C149"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>